<commit_message>
se elimina segementacione horizontales y verticales al cerrar SelectAreas. Listo para estimar
</commit_message>
<xml_diff>
--- a/Uso memoria intensivo.xlsx
+++ b/Uso memoria intensivo.xlsx
@@ -24,12 +24,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Total Dicoms</t>
   </si>
   <si>
     <t>RAM Megas</t>
+  </si>
+  <si>
+    <t>sin Low</t>
   </si>
 </sst>
 </file>
@@ -265,6 +268,121 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.715071574957241E-2"/>
+                  <c:y val="-7.1722440944881893E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-CO"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$E$2:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$F$2:$F$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1740</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2070</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -273,11 +391,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="417606824"/>
-        <c:axId val="198860104"/>
+        <c:axId val="249880552"/>
+        <c:axId val="249986624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="417606824"/>
+        <c:axId val="249880552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -334,12 +452,12 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="198860104"/>
+        <c:crossAx val="249986624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="198860104"/>
+        <c:axId val="249986624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -396,7 +514,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="417606824"/>
+        <c:crossAx val="249880552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1299,10 +1417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C6"/>
+  <dimension ref="B1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="B1:C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,39 +1428,63 @@
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>600</v>
       </c>
       <c r="C2">
         <v>1840</v>
       </c>
+      <c r="E2">
+        <v>300</v>
+      </c>
+      <c r="F2">
+        <v>1200</v>
+      </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1000</v>
       </c>
       <c r="C3">
         <v>3050</v>
       </c>
+      <c r="E3">
+        <v>500</v>
+      </c>
+      <c r="F3">
+        <v>1740</v>
+      </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1400</v>
       </c>
       <c r="C4">
         <v>3870</v>
       </c>
+      <c r="E4">
+        <v>700</v>
+      </c>
+      <c r="F4">
+        <v>2070</v>
+      </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1800</v>
       </c>
@@ -1350,7 +1492,7 @@
         <v>4380</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2200</v>
       </c>

</xml_diff>